<commit_message>
update diem de tai
</commit_message>
<xml_diff>
--- a/NCKH-QLDA/src/WebSite.Core.API/uploadsAPIQLDA/Điểm phản biện/2021/06/28/62483e655c574f3bb673ade600ba1c9c.xlsx
+++ b/NCKH-QLDA/src/WebSite.Core.API/uploadsAPIQLDA/Điểm phản biện/2021/06/28/62483e655c574f3bb673ade600ba1c9c.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="DiemPhanBien" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -133,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -296,8 +297,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H8">
-  <autoFilter ref="A1:H8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H9">
+  <autoFilter ref="A2:H9"/>
   <tableColumns count="8">
     <tableColumn id="1" name="IdPhanBien"/>
     <tableColumn id="2" name="Diem" dataDxfId="1"/>
@@ -578,207 +579,206 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="40" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.5703125" style="3" customWidth="1"/>
     <col min="2" max="16383" width="40" style="4" customWidth="1"/>
     <col min="16384" max="16384" width="40" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8 16384:16384" s="1" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="XFD1" s="7"/>
+    </row>
+    <row r="2" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="XFD1" s="7"/>
-    </row>
-    <row r="2" spans="1:8 16384:16384" ht="30">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:8 16384:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B3" s="10">
         <v>8.5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8 16384:16384" ht="30">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="10">
-        <v>8.9</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8 16384:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="10">
+        <v>8.9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H4" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8 16384:16384">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B5" s="10">
         <v>8.4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H5" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8 16384:16384" ht="30">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:8 16384:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="10">
-        <v>9.5</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8 16384:16384">
-      <c r="A6" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="B6" s="10">
         <v>9.5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8 16384:16384" ht="30">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:8 16384:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B8" s="10">
         <v>8</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8 16384:16384">
-      <c r="A8" s="3">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="1048576" spans="1:1 16384:16384" s="2" customFormat="1">
+    <row r="9" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="1048576" spans="1:1 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1048576" s="8"/>
       <c r="XFD1048576" s="9"/>
     </row>
@@ -788,4 +788,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>